<commit_message>
Desisti! não consegui burlar o HCAPTCHA
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADM\Desktop\PROJETOS\EmissaoGuiasPy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4256E671-6ABC-4CD2-887A-C0D410B3F61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91770823-C38E-4A4C-9FCF-25629ECD6181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{9DFDB11D-7ED0-4833-A880-3973C6660404}"/>
+    <workbookView xWindow="30075" yWindow="1290" windowWidth="17250" windowHeight="8865" xr2:uid="{9DFDB11D-7ED0-4833-A880-3973C6660404}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -424,7 +424,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,7 +449,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="4">
-        <v>41949858000184</v>
+        <v>11008634000107</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -460,7 +460,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>41949858000184</v>
+        <v>11008634000107</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>

</xml_diff>